<commit_message>
Add logging in log.txt
</commit_message>
<xml_diff>
--- a/commands.xlsx
+++ b/commands.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="commands" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="times" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="schedule" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="users" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="commands" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="times" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="schedule" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="users" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -780,7 +780,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="A2:B3"/>
@@ -814,6 +814,16 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>108127462</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>